<commit_message>
bump ktor to 2.2.2 & auto refactoring
</commit_message>
<xml_diff>
--- a/backend/src/test/resources/routes/xml/source.xlsx
+++ b/backend/src/test/resources/routes/xml/source.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\kotlin\AlfaConverter\backend\src\test\resources\modules\xml\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\kotlin\AlfaConverter\backend\src\test\resources\routes\xml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4223D5-93EF-48B9-B765-74492C5307E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE72EBC7-EC55-4548-BB2E-AFC2D0407A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18555" yWindow="1380" windowWidth="17595" windowHeight="10965" xr2:uid="{4FFCCFEC-BF92-4A12-94D8-B011486D6CEA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4FFCCFEC-BF92-4A12-94D8-B011486D6CEA}"/>
   </bookViews>
   <sheets>
     <sheet name="исходный формат" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Клинико-диагностический центр</t>
   </si>
@@ -99,6 +99,27 @@
   </si>
   <si>
     <t>Возраст пациента</t>
+  </si>
+  <si>
+    <t>Петров Пётр Петрович</t>
+  </si>
+  <si>
+    <t>Пушкина 12</t>
+  </si>
+  <si>
+    <t>В23-32</t>
+  </si>
+  <si>
+    <t>Склероз</t>
+  </si>
+  <si>
+    <t>Обыкновенное</t>
+  </si>
+  <si>
+    <t>Пушкина 13</t>
+  </si>
+  <si>
+    <t>Лучшая лаборатория мира</t>
   </si>
 </sst>
 </file>
@@ -142,7 +163,7 @@
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -158,9 +179,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -198,7 +219,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -304,7 +325,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -454,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1500AA-4EF8-4E68-9C39-0CBF91E29FFA}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,6 +486,7 @@
     <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -557,6 +579,50 @@
         <v>0.57847222222222217</v>
       </c>
     </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="2">
+        <v>114303</v>
+      </c>
+      <c r="C3">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3" s="2">
+        <v>114304</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="M3" s="2">
+        <v>114305</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0.95833333333333337</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>